<commit_message>
Second bug with friends detailed list fixed
Updated profile styles
</commit_message>
<xml_diff>
--- a/Level-2/JS-Frameworks-with-AngularJS/Social-Network-Project/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/Level-2/JS-Frameworks-with-AngularJS/Social-Network-Project/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>